<commit_message>
Fixed inconsistency in Source.xlsx regarding lake storage capacity
</commit_message>
<xml_diff>
--- a/Sources.xlsx
+++ b/Sources.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hippo\Documents\CIRED\Eoles\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA4F06F-C018-4927-8D6E-B5340392F1D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Costs" sheetId="7" r:id="rId1"/>
@@ -21,7 +15,7 @@
     <sheet name="Technology characteristics" sheetId="14" r:id="rId6"/>
     <sheet name="Production profiles" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="145621" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="324">
   <si>
     <t>Source</t>
   </si>
@@ -971,9 +965,6 @@
     <t>https://www.services-rte.com/fr/visualisez-les-donnees-publiees-par-rte/stock-hydraulique.html gives a slightly different number</t>
   </si>
   <si>
-    <t>A préciser</t>
-  </si>
-  <si>
     <t>SNBC (à préciser)</t>
   </si>
   <si>
@@ -1038,12 +1029,20 @@
   </si>
   <si>
     <t>La partie de la demande concernant le chauffage et la climatisation des bâtiments résidentiels, industriels et tertiaires a été isolée de la demande négaWatt (sont enlevés du compte les groupes : 1, 4, 10, 13, 36, 39, 40, 41), dans le but d'assurer une cohérence entre la demande thermosensible et la production renouvelable. Pour la chaleur, la valeur de la consommation annuelle prévue par négaWatt a été répartie selon le profil des HDD de 2000 à 2018 obtenu sur renewables.ninja (valeurs journalières de HDD réparties selon un profil horaire de consommation). Le profil intra-journalier (horaire) de répartition de la demande de chaleur est obtenu en effectuant le ratio entre le profil 2019 calculé avec profil intra-journalier et sans (case "Use diurnal profile"), pour les données horaires fournies par renewables.ninja en 2019 (le profil obtenu est quasimment identique chaque jour, la moyenne annuelle a été prise). Pour la climatisation, pour des raisons expliquées dans l'article, nous utilisons le profil journalier de CDD de renewables.ninja et les pentes de climatisation de RTE, ainsi que le profil de répartition intra-journalier (horaire) obtenu à partir des estimations de consommation de 2020 du tertiaire réalisées en 2015 par RTE (profil identique chaque jour, extrait à partir de la consommation).</t>
+  </si>
+  <si>
+    <t>OpenData Réseaux Energie : Registre
+national des installations de production et de stockage d’électricité (au
+31/03/2024)</t>
+  </si>
+  <si>
+    <t>ocgt, ocgt_coge</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1133,7 +1132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1177,6 +1176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1204,7 +1204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,7 +1228,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
@@ -1421,7 +1426,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5CAB-43D8-B1F6-CB228DF2248F}"/>
             </c:ext>
@@ -1435,11 +1440,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1094557120"/>
-        <c:axId val="1094563360"/>
+        <c:axId val="190528896"/>
+        <c:axId val="190547072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1094557120"/>
+        <c:axId val="190528896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1496,12 +1501,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1094563360"/>
+        <c:crossAx val="190547072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1094563360"/>
+        <c:axId val="190547072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1563,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1094557120"/>
+        <c:crossAx val="190528896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1572,14 +1577,14 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2190,7 +2195,7 @@
         <xdr:cNvPr id="2" name="Graphique 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D647604-B4B0-9371-D708-B64637B0BBAB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6D647604-B4B0-9371-D708-B64637B0BBAB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2231,7 +2236,7 @@
         <xdr:cNvPr id="3" name="Image 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AAF58FE-6B52-A4C9-9AE6-D07B727E136D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4AAF58FE-6B52-A4C9-9AE6-D07B727E136D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2281,7 +2286,7 @@
         <xdr:cNvPr id="5" name="Image 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4BF55DA-E3C8-2D62-2572-E41804A5B8E1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C4BF55DA-E3C8-2D62-2572-E41804A5B8E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2571,17 +2576,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5747FAFC-21A4-4E39-8800-9F6AE1CDA773}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T130"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D139" sqref="D139"/>
     </sheetView>
   </sheetViews>
@@ -2622,7 +2627,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -2649,7 +2654,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
@@ -2703,7 +2708,7 @@
       <c r="E10" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="20" t="s">
         <v>176</v>
       </c>
     </row>
@@ -2717,7 +2722,7 @@
       <c r="E11" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
@@ -2730,25 +2735,25 @@
         <v>173</v>
       </c>
       <c r="F12" s="13"/>
-      <c r="N12" s="28" t="s">
+      <c r="N12" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="O12" s="28" t="s">
+      <c r="O12" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="P12" s="28" t="s">
+      <c r="P12" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="Q12" s="28" t="s">
+      <c r="Q12" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="R12" s="28" t="s">
+      <c r="R12" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="S12" s="28" t="s">
+      <c r="S12" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="T12" s="28" t="s">
+      <c r="T12" s="19" t="s">
         <v>167</v>
       </c>
     </row>
@@ -3305,7 +3310,7 @@
       <c r="E52" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F52" s="19" t="s">
+      <c r="F52" s="20" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3319,7 +3324,7 @@
       <c r="E53" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F53" s="19"/>
+      <c r="F53" s="20"/>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="5" t="s">
@@ -3506,11 +3511,11 @@
       <c r="C69" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E69" s="20" t="s">
+      <c r="E69" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="F69" s="12" t="s">
         <v>319</v>
-      </c>
-      <c r="F69" s="12" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -3520,9 +3525,9 @@
       <c r="C70" t="s">
         <v>17</v>
       </c>
-      <c r="E70" s="21"/>
+      <c r="E70" s="22"/>
       <c r="F70" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="71" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -3676,7 +3681,7 @@
       <c r="E83" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F83" s="19" t="s">
+      <c r="F83" s="20" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3690,7 +3695,7 @@
       <c r="E84" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F84" s="19"/>
+      <c r="F84" s="20"/>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="5" t="s">
@@ -4011,7 +4016,7 @@
       <c r="E112" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F112" s="19" t="s">
+      <c r="F112" s="20" t="s">
         <v>176</v>
       </c>
     </row>
@@ -4025,7 +4030,7 @@
       <c r="E113" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="F113" s="19"/>
+      <c r="F113" s="20"/>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B114" s="5" t="s">
@@ -4239,7 +4244,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48C8C87-56DC-4732-952A-57FA308F4E83}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4321,7 +4326,7 @@
         <v>280</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -4330,11 +4335,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E4F1-E9B2-440D-AAB9-55E90FA2E8D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4468,38 +4473,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="10" customFormat="1" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>84</v>
       </c>
       <c r="D10" s="10">
         <v>3819.3</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="10" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="10">
         <v>101</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>300</v>
-      </c>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="F10:F11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F949D6-08AB-49F3-BE6E-760233317217}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4596,10 +4604,10 @@
       <c r="D6" s="12">
         <v>0.01</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="20" t="s">
         <v>197</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="23" t="s">
         <v>198</v>
       </c>
     </row>
@@ -4613,8 +4621,8 @@
       <c r="D7">
         <v>0.1</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -4696,10 +4704,10 @@
         <v>250</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D14" s="12">
         <v>1.8899999999999999E-5</v>
@@ -4708,7 +4716,7 @@
         <v>251</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -4728,7 +4736,7 @@
         <v>255</v>
       </c>
       <c r="F15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -4781,11 +4789,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BCEB52-9CFB-4E56-9D31-3F8E8F833F98}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5059,10 +5067,10 @@
       <c r="D21" s="15">
         <v>1.6199999999999999E-3</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="26" t="s">
         <v>218</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="24" t="s">
         <v>182</v>
       </c>
     </row>
@@ -5079,8 +5087,8 @@
       <c r="D22" s="8">
         <v>6.5799999999999999E-3</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="24"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
@@ -5186,7 +5194,7 @@
         <v>84</v>
       </c>
       <c r="D32">
-        <v>3591</v>
+        <v>3819.3</v>
       </c>
       <c r="E32" t="s">
         <v>214</v>
@@ -5202,11 +5210,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DFEBD0-1F26-470C-9238-D32313B047C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="C50" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5509,7 +5517,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -5520,7 +5528,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -5531,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -5542,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -5553,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -5564,7 +5572,7 @@
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
@@ -5608,7 +5616,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>221</v>
+        <v>323</v>
       </c>
       <c r="D32">
         <v>0.4</v>
@@ -5646,7 +5654,7 @@
         <v>189</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -5863,7 +5871,7 @@
         <v>283</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -5936,10 +5944,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E667736-E036-4736-90C6-30487663045B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -5972,7 +5980,7 @@
     </row>
     <row r="2" spans="1:5" ht="30.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>46</v>
@@ -5986,7 +5994,7 @@
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>47</v>
@@ -6034,7 +6042,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>48</v>
@@ -6073,7 +6081,7 @@
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>57</v>
@@ -6084,13 +6092,13 @@
       <c r="D9" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="21" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>57</v>
@@ -6101,11 +6109,11 @@
       <c r="D10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="28"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>57</v>
@@ -6116,11 +6124,11 @@
       <c r="D11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>57</v>
@@ -6129,12 +6137,12 @@
         <v>32</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>57</v>
@@ -6143,12 +6151,12 @@
         <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>57</v>

</xml_diff>